<commit_message>
fix issue of converting factors to numeric before creating plots
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,7 +440,7 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.9290000000000001</v>
+        <v>0.929</v>
       </c>
       <c r="D2">
         <v>0.6870000000000001</v>
@@ -507,7 +507,7 @@
         <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="K3">
         <v>0.6870000000000001</v>
@@ -581,10 +581,10 @@
         <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="E5">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="F5">
         <v>0.863</v>
@@ -596,7 +596,7 @@
         <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="J5">
         <v>0.879</v>
@@ -639,19 +639,19 @@
         <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I6">
         <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.5550000000000001</v>
+        <v>0.555</v>
       </c>
       <c r="K6">
         <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="M6">
         <v>0.387</v>
@@ -676,13 +676,13 @@
         <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="F7">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G7">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="H7">
         <v>0.707</v>
@@ -691,10 +691,10 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="K7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="L7">
         <v>0.709</v>
@@ -955,7 +955,7 @@
         <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="G13">
         <v>0.903</v>
@@ -970,7 +970,7 @@
         <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="L13">
         <v>0.661</v>
@@ -1041,16 +1041,16 @@
         <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E15">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F15">
         <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="H15">
         <v>0.879</v>
@@ -1087,7 +1087,7 @@
         <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E16">
         <v>0.898</v>
@@ -1194,7 +1194,7 @@
         <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J18">
         <v>0.909</v>
@@ -1234,7 +1234,7 @@
         <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="H19">
         <v>0.821</v>
@@ -1280,10 +1280,10 @@
         <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H20">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="I20">
         <v>0.716</v>
@@ -1317,7 +1317,7 @@
         <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E21">
         <v>0.767</v>
@@ -1452,13 +1452,13 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="D24">
         <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.5540000000000001</v>
+        <v>0.554</v>
       </c>
       <c r="F24">
         <v>0.75</v>
@@ -1470,7 +1470,7 @@
         <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="J24">
         <v>0.883</v>
@@ -1636,7 +1636,7 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D28">
         <v>0.919</v>
@@ -1654,7 +1654,7 @@
         <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="J28">
         <v>0.916</v>
@@ -1691,7 +1691,7 @@
         <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="G29">
         <v>0.763</v>
@@ -1749,7 +1749,7 @@
         <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="K30">
         <v>0.712</v>
@@ -1792,7 +1792,7 @@
         <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.689</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="J31">
         <v>0.787</v>
@@ -1832,7 +1832,7 @@
         <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="H32">
         <v>0.701</v>
@@ -1884,7 +1884,7 @@
         <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J33">
         <v>0.731</v>
@@ -2111,7 +2111,7 @@
         <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="I38">
         <v>0.881</v>
@@ -2160,7 +2160,7 @@
         <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J39">
         <v>0.718</v>
@@ -2172,7 +2172,7 @@
         <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="N39">
         <v>0.267</v>
@@ -2206,7 +2206,7 @@
         <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J40">
         <v>0.9</v>
@@ -2237,7 +2237,7 @@
         <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="E41">
         <v>0.852</v>
@@ -2326,7 +2326,7 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="D43">
         <v>0.773</v>
@@ -2372,7 +2372,7 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D44">
         <v>0.907</v>
@@ -2384,7 +2384,7 @@
         <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="H44">
         <v>0.9</v>
@@ -2433,7 +2433,7 @@
         <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I45">
         <v>0.858</v>
@@ -2470,10 +2470,10 @@
         <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="F46">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="G46">
         <v>0.9360000000000001</v>
@@ -2491,13 +2491,13 @@
         <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="M46">
         <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.5510000000000001</v>
+        <v>0.551</v>
       </c>
     </row>
     <row r="47">
@@ -2666,7 +2666,7 @@
         <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="J50">
         <v>0.828</v>
@@ -2740,7 +2740,7 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D52">
         <v>0.836</v>
@@ -2755,7 +2755,7 @@
         <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="I52">
         <v>0.821</v>
@@ -2792,7 +2792,7 @@
         <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="F53">
         <v>0.626</v>
@@ -2801,7 +2801,7 @@
         <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I53">
         <v>0.754</v>
@@ -2832,7 +2832,7 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D54">
         <v>0.903</v>
@@ -2850,7 +2850,7 @@
         <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="J54">
         <v>0.76</v>
@@ -2862,7 +2862,7 @@
         <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.565</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="N54">
         <v>0.387</v>
@@ -2884,7 +2884,7 @@
         <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F55">
         <v>0.745</v>
@@ -2893,7 +2893,7 @@
         <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="I55">
         <v>0.891</v>
@@ -2924,7 +2924,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="D56">
         <v>0.754</v>
@@ -2979,7 +2979,7 @@
         <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="G57">
         <v>0.748</v>
@@ -3025,7 +3025,7 @@
         <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="G58">
         <v>0.761</v>
@@ -3126,10 +3126,10 @@
         <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J60">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="K60">
         <v>0.785</v>
@@ -3172,7 +3172,7 @@
         <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="J61">
         <v>0.784</v>
@@ -3298,7 +3298,7 @@
         <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.8030000000000001</v>
+        <v>0.803</v>
       </c>
       <c r="F64">
         <v>0.834</v>
@@ -3359,7 +3359,7 @@
         <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="K65">
         <v>0.668</v>
@@ -3457,7 +3457,7 @@
         <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="M67">
         <v>0.362</v>
@@ -3500,7 +3500,7 @@
         <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="L68">
         <v>0.697</v>
@@ -3522,7 +3522,7 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D69">
         <v>0.8110000000000001</v>
@@ -3592,7 +3592,7 @@
         <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.692</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="L70">
         <v>0.529</v>
@@ -3632,7 +3632,7 @@
         <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J71">
         <v>0.92</v>
@@ -3663,7 +3663,7 @@
         <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E72">
         <v>0.907</v>
@@ -3681,7 +3681,7 @@
         <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="K72">
         <v>0.861</v>
@@ -3690,7 +3690,7 @@
         <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.5530000000000001</v>
+        <v>0.553</v>
       </c>
       <c r="N72">
         <v>0.387</v>
@@ -3718,7 +3718,7 @@
         <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="H73">
         <v>0.891</v>
@@ -3758,10 +3758,10 @@
         <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F74">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G74">
         <v>0.921</v>
@@ -3776,7 +3776,7 @@
         <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="L74">
         <v>0.734</v>
@@ -3871,7 +3871,7 @@
         <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M76">
         <v>0.5629999999999999</v>
@@ -3902,7 +3902,7 @@
         <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.8020000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="H77">
         <v>0.791</v>
@@ -3942,7 +3942,7 @@
         <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="F78">
         <v>0.821</v>
@@ -3960,10 +3960,10 @@
         <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="L78">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M78">
         <v>0.454</v>
@@ -3988,7 +3988,7 @@
         <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="F79">
         <v>0.836</v>
@@ -4031,7 +4031,7 @@
         <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="E80">
         <v>0.872</v>
@@ -4098,7 +4098,7 @@
         <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.693</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="L81">
         <v>0.536</v>
@@ -4193,7 +4193,7 @@
         <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.5560000000000001</v>
+        <v>0.556</v>
       </c>
       <c r="M83">
         <v>0.344</v>
@@ -4399,13 +4399,13 @@
         <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="E88">
         <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G88">
         <v>0.949</v>
@@ -4414,7 +4414,7 @@
         <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="J88">
         <v>0.825</v>
@@ -4506,7 +4506,7 @@
         <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J90">
         <v>0.772</v>
@@ -4515,7 +4515,7 @@
         <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="M90">
         <v>0.595</v>

</xml_diff>

<commit_message>
edits to code to remove warnings
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,7 +440,7 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.9290000000000001</v>
+        <v>0.929</v>
       </c>
       <c r="D2">
         <v>0.6870000000000001</v>
@@ -507,7 +507,7 @@
         <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="K3">
         <v>0.6870000000000001</v>
@@ -581,10 +581,10 @@
         <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="E5">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="F5">
         <v>0.863</v>
@@ -596,7 +596,7 @@
         <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="J5">
         <v>0.879</v>
@@ -639,19 +639,19 @@
         <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I6">
         <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.5550000000000001</v>
+        <v>0.555</v>
       </c>
       <c r="K6">
         <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="M6">
         <v>0.387</v>
@@ -676,13 +676,13 @@
         <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="F7">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G7">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="H7">
         <v>0.707</v>
@@ -691,10 +691,10 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="K7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="L7">
         <v>0.709</v>
@@ -955,7 +955,7 @@
         <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="G13">
         <v>0.903</v>
@@ -970,7 +970,7 @@
         <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="L13">
         <v>0.661</v>
@@ -1041,16 +1041,16 @@
         <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E15">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F15">
         <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="H15">
         <v>0.879</v>
@@ -1087,7 +1087,7 @@
         <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E16">
         <v>0.898</v>
@@ -1194,7 +1194,7 @@
         <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J18">
         <v>0.909</v>
@@ -1234,7 +1234,7 @@
         <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="H19">
         <v>0.821</v>
@@ -1280,10 +1280,10 @@
         <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H20">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="I20">
         <v>0.716</v>
@@ -1317,7 +1317,7 @@
         <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E21">
         <v>0.767</v>
@@ -1452,13 +1452,13 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="D24">
         <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.5540000000000001</v>
+        <v>0.554</v>
       </c>
       <c r="F24">
         <v>0.75</v>
@@ -1470,7 +1470,7 @@
         <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="J24">
         <v>0.883</v>
@@ -1636,7 +1636,7 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D28">
         <v>0.919</v>
@@ -1654,7 +1654,7 @@
         <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="J28">
         <v>0.916</v>
@@ -1691,7 +1691,7 @@
         <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="G29">
         <v>0.763</v>
@@ -1749,7 +1749,7 @@
         <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="K30">
         <v>0.712</v>
@@ -1792,7 +1792,7 @@
         <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.689</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="J31">
         <v>0.787</v>
@@ -1832,7 +1832,7 @@
         <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="H32">
         <v>0.701</v>
@@ -1884,7 +1884,7 @@
         <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J33">
         <v>0.731</v>
@@ -2111,7 +2111,7 @@
         <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="I38">
         <v>0.881</v>
@@ -2160,7 +2160,7 @@
         <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J39">
         <v>0.718</v>
@@ -2172,7 +2172,7 @@
         <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="N39">
         <v>0.267</v>
@@ -2206,7 +2206,7 @@
         <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J40">
         <v>0.9</v>
@@ -2237,7 +2237,7 @@
         <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="E41">
         <v>0.852</v>
@@ -2326,7 +2326,7 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="D43">
         <v>0.773</v>
@@ -2372,7 +2372,7 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D44">
         <v>0.907</v>
@@ -2384,7 +2384,7 @@
         <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="H44">
         <v>0.9</v>
@@ -2433,7 +2433,7 @@
         <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I45">
         <v>0.858</v>
@@ -2470,10 +2470,10 @@
         <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="F46">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="G46">
         <v>0.9360000000000001</v>
@@ -2491,13 +2491,13 @@
         <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="M46">
         <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.5510000000000001</v>
+        <v>0.551</v>
       </c>
     </row>
     <row r="47">
@@ -2666,7 +2666,7 @@
         <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="J50">
         <v>0.828</v>
@@ -2740,7 +2740,7 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D52">
         <v>0.836</v>
@@ -2755,7 +2755,7 @@
         <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="I52">
         <v>0.821</v>
@@ -2792,7 +2792,7 @@
         <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="F53">
         <v>0.626</v>
@@ -2801,7 +2801,7 @@
         <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I53">
         <v>0.754</v>
@@ -2832,7 +2832,7 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D54">
         <v>0.903</v>
@@ -2850,7 +2850,7 @@
         <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="J54">
         <v>0.76</v>
@@ -2862,7 +2862,7 @@
         <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.565</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="N54">
         <v>0.387</v>
@@ -2884,7 +2884,7 @@
         <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F55">
         <v>0.745</v>
@@ -2893,7 +2893,7 @@
         <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="I55">
         <v>0.891</v>
@@ -2924,7 +2924,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="D56">
         <v>0.754</v>
@@ -2979,7 +2979,7 @@
         <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="G57">
         <v>0.748</v>
@@ -3025,7 +3025,7 @@
         <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="G58">
         <v>0.761</v>
@@ -3126,10 +3126,10 @@
         <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J60">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="K60">
         <v>0.785</v>
@@ -3172,7 +3172,7 @@
         <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="J61">
         <v>0.784</v>
@@ -3298,7 +3298,7 @@
         <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.8030000000000001</v>
+        <v>0.803</v>
       </c>
       <c r="F64">
         <v>0.834</v>
@@ -3359,7 +3359,7 @@
         <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="K65">
         <v>0.668</v>
@@ -3457,7 +3457,7 @@
         <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="M67">
         <v>0.362</v>
@@ -3500,7 +3500,7 @@
         <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="L68">
         <v>0.697</v>
@@ -3522,7 +3522,7 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D69">
         <v>0.8110000000000001</v>
@@ -3592,7 +3592,7 @@
         <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.692</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="L70">
         <v>0.529</v>
@@ -3632,7 +3632,7 @@
         <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J71">
         <v>0.92</v>
@@ -3663,7 +3663,7 @@
         <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E72">
         <v>0.907</v>
@@ -3681,7 +3681,7 @@
         <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="K72">
         <v>0.861</v>
@@ -3690,7 +3690,7 @@
         <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.5530000000000001</v>
+        <v>0.553</v>
       </c>
       <c r="N72">
         <v>0.387</v>
@@ -3718,7 +3718,7 @@
         <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="H73">
         <v>0.891</v>
@@ -3758,10 +3758,10 @@
         <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F74">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G74">
         <v>0.921</v>
@@ -3776,7 +3776,7 @@
         <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="L74">
         <v>0.734</v>
@@ -3871,7 +3871,7 @@
         <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M76">
         <v>0.5629999999999999</v>
@@ -3902,7 +3902,7 @@
         <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.8020000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="H77">
         <v>0.791</v>
@@ -3942,7 +3942,7 @@
         <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="F78">
         <v>0.821</v>
@@ -3960,10 +3960,10 @@
         <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="L78">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M78">
         <v>0.454</v>
@@ -3988,7 +3988,7 @@
         <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="F79">
         <v>0.836</v>
@@ -4031,7 +4031,7 @@
         <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="E80">
         <v>0.872</v>
@@ -4098,7 +4098,7 @@
         <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.693</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="L81">
         <v>0.536</v>
@@ -4193,7 +4193,7 @@
         <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.5560000000000001</v>
+        <v>0.556</v>
       </c>
       <c r="M83">
         <v>0.344</v>
@@ -4399,13 +4399,13 @@
         <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="E88">
         <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G88">
         <v>0.949</v>
@@ -4414,7 +4414,7 @@
         <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="J88">
         <v>0.825</v>
@@ -4506,7 +4506,7 @@
         <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J90">
         <v>0.772</v>
@@ -4515,7 +4515,7 @@
         <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="M90">
         <v>0.595</v>

</xml_diff>

<commit_message>
read in gdp data, create four variables and join to existing data
</commit_message>
<xml_diff>
--- a/clean-data/output/citizenship-norm-indicator-tables.xlsx
+++ b/clean-data/output/citizenship-norm-indicator-tables.xlsx
@@ -440,7 +440,7 @@
         <v>1999</v>
       </c>
       <c r="C2">
-        <v>0.9290000000000001</v>
+        <v>0.929</v>
       </c>
       <c r="D2">
         <v>0.6870000000000001</v>
@@ -507,7 +507,7 @@
         <v>0.772</v>
       </c>
       <c r="J3">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="K3">
         <v>0.6870000000000001</v>
@@ -581,10 +581,10 @@
         <v>0.9340000000000001</v>
       </c>
       <c r="D5">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="E5">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="F5">
         <v>0.863</v>
@@ -596,7 +596,7 @@
         <v>0.846</v>
       </c>
       <c r="I5">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="J5">
         <v>0.879</v>
@@ -639,19 +639,19 @@
         <v>0.72</v>
       </c>
       <c r="H6">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I6">
         <v>0.419</v>
       </c>
       <c r="J6">
-        <v>0.5550000000000001</v>
+        <v>0.555</v>
       </c>
       <c r="K6">
         <v>0.579</v>
       </c>
       <c r="L6">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="M6">
         <v>0.387</v>
@@ -676,13 +676,13 @@
         <v>0.823</v>
       </c>
       <c r="E7">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="F7">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G7">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="H7">
         <v>0.707</v>
@@ -691,10 +691,10 @@
         <v>0.799</v>
       </c>
       <c r="J7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="K7">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="L7">
         <v>0.709</v>
@@ -955,7 +955,7 @@
         <v>0.903</v>
       </c>
       <c r="F13">
-        <v>0.8040000000000001</v>
+        <v>0.804</v>
       </c>
       <c r="G13">
         <v>0.903</v>
@@ -970,7 +970,7 @@
         <v>0.849</v>
       </c>
       <c r="K13">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="L13">
         <v>0.661</v>
@@ -1041,16 +1041,16 @@
         <v>0.974</v>
       </c>
       <c r="D15">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E15">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F15">
         <v>0.837</v>
       </c>
       <c r="G15">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="H15">
         <v>0.879</v>
@@ -1087,7 +1087,7 @@
         <v>0.875</v>
       </c>
       <c r="D16">
-        <v>0.941</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="E16">
         <v>0.898</v>
@@ -1194,7 +1194,7 @@
         <v>0.914</v>
       </c>
       <c r="I18">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J18">
         <v>0.909</v>
@@ -1234,7 +1234,7 @@
         <v>0.718</v>
       </c>
       <c r="G19">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="H19">
         <v>0.821</v>
@@ -1280,10 +1280,10 @@
         <v>0.772</v>
       </c>
       <c r="G20">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="H20">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="I20">
         <v>0.716</v>
@@ -1317,7 +1317,7 @@
         <v>0.922</v>
       </c>
       <c r="D21">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E21">
         <v>0.767</v>
@@ -1452,13 +1452,13 @@
         <v>2009</v>
       </c>
       <c r="C24">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="D24">
         <v>0.6879999999999999</v>
       </c>
       <c r="E24">
-        <v>0.5540000000000001</v>
+        <v>0.554</v>
       </c>
       <c r="F24">
         <v>0.75</v>
@@ -1470,7 +1470,7 @@
         <v>0.791</v>
       </c>
       <c r="I24">
-        <v>0.6770000000000001</v>
+        <v>0.677</v>
       </c>
       <c r="J24">
         <v>0.883</v>
@@ -1636,7 +1636,7 @@
         <v>2016</v>
       </c>
       <c r="C28">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D28">
         <v>0.919</v>
@@ -1654,7 +1654,7 @@
         <v>0.77</v>
       </c>
       <c r="I28">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="J28">
         <v>0.916</v>
@@ -1691,7 +1691,7 @@
         <v>0.785</v>
       </c>
       <c r="F29">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="G29">
         <v>0.763</v>
@@ -1749,7 +1749,7 @@
         <v>0.628</v>
       </c>
       <c r="J30">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="K30">
         <v>0.712</v>
@@ -1792,7 +1792,7 @@
         <v>0.761</v>
       </c>
       <c r="I31">
-        <v>0.689</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="J31">
         <v>0.787</v>
@@ -1832,7 +1832,7 @@
         <v>0.827</v>
       </c>
       <c r="G32">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="H32">
         <v>0.701</v>
@@ -1884,7 +1884,7 @@
         <v>0.669</v>
       </c>
       <c r="I33">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J33">
         <v>0.731</v>
@@ -2111,7 +2111,7 @@
         <v>0.888</v>
       </c>
       <c r="H38">
-        <v>0.943</v>
+        <v>0.9429999999999999</v>
       </c>
       <c r="I38">
         <v>0.881</v>
@@ -2160,7 +2160,7 @@
         <v>0.747</v>
       </c>
       <c r="I39">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J39">
         <v>0.718</v>
@@ -2172,7 +2172,7 @@
         <v>0.778</v>
       </c>
       <c r="M39">
-        <v>0.568</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="N39">
         <v>0.267</v>
@@ -2206,7 +2206,7 @@
         <v>0.922</v>
       </c>
       <c r="I40">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="J40">
         <v>0.9</v>
@@ -2237,7 +2237,7 @@
         <v>0.944</v>
       </c>
       <c r="D41">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="E41">
         <v>0.852</v>
@@ -2326,7 +2326,7 @@
         <v>2016</v>
       </c>
       <c r="C43">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="D43">
         <v>0.773</v>
@@ -2372,7 +2372,7 @@
         <v>2016</v>
       </c>
       <c r="C44">
-        <v>0.942</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="D44">
         <v>0.907</v>
@@ -2384,7 +2384,7 @@
         <v>0.953</v>
       </c>
       <c r="G44">
-        <v>0.9270000000000001</v>
+        <v>0.927</v>
       </c>
       <c r="H44">
         <v>0.9</v>
@@ -2433,7 +2433,7 @@
         <v>0.765</v>
       </c>
       <c r="H45">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="I45">
         <v>0.858</v>
@@ -2470,10 +2470,10 @@
         <v>0.857</v>
       </c>
       <c r="E46">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="F46">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="G46">
         <v>0.9360000000000001</v>
@@ -2491,13 +2491,13 @@
         <v>0.743</v>
       </c>
       <c r="L46">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="M46">
         <v>0.482</v>
       </c>
       <c r="N46">
-        <v>0.5510000000000001</v>
+        <v>0.551</v>
       </c>
     </row>
     <row r="47">
@@ -2666,7 +2666,7 @@
         <v>0.91</v>
       </c>
       <c r="I50">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="J50">
         <v>0.828</v>
@@ -2740,7 +2740,7 @@
         <v>2016</v>
       </c>
       <c r="C52">
-        <v>0.939</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="D52">
         <v>0.836</v>
@@ -2755,7 +2755,7 @@
         <v>0.898</v>
       </c>
       <c r="H52">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="I52">
         <v>0.821</v>
@@ -2792,7 +2792,7 @@
         <v>0.714</v>
       </c>
       <c r="E53">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="F53">
         <v>0.626</v>
@@ -2801,7 +2801,7 @@
         <v>0.652</v>
       </c>
       <c r="H53">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I53">
         <v>0.754</v>
@@ -2832,7 +2832,7 @@
         <v>1999</v>
       </c>
       <c r="C54">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D54">
         <v>0.903</v>
@@ -2850,7 +2850,7 @@
         <v>0.839</v>
       </c>
       <c r="I54">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="J54">
         <v>0.76</v>
@@ -2862,7 +2862,7 @@
         <v>0.721</v>
       </c>
       <c r="M54">
-        <v>0.565</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="N54">
         <v>0.387</v>
@@ -2884,7 +2884,7 @@
         <v>0.765</v>
       </c>
       <c r="E55">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="F55">
         <v>0.745</v>
@@ -2893,7 +2893,7 @@
         <v>0.771</v>
       </c>
       <c r="H55">
-        <v>0.8060000000000001</v>
+        <v>0.806</v>
       </c>
       <c r="I55">
         <v>0.891</v>
@@ -2924,7 +2924,7 @@
         <v>2016</v>
       </c>
       <c r="C56">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="D56">
         <v>0.754</v>
@@ -2979,7 +2979,7 @@
         <v>0.665</v>
       </c>
       <c r="F57">
-        <v>0.6790000000000001</v>
+        <v>0.679</v>
       </c>
       <c r="G57">
         <v>0.748</v>
@@ -3025,7 +3025,7 @@
         <v>0.726</v>
       </c>
       <c r="F58">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="G58">
         <v>0.761</v>
@@ -3126,10 +3126,10 @@
         <v>0.791</v>
       </c>
       <c r="I60">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="J60">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="K60">
         <v>0.785</v>
@@ -3172,7 +3172,7 @@
         <v>0.87</v>
       </c>
       <c r="I61">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="J61">
         <v>0.784</v>
@@ -3298,7 +3298,7 @@
         <v>0.849</v>
       </c>
       <c r="E64">
-        <v>0.8030000000000001</v>
+        <v>0.803</v>
       </c>
       <c r="F64">
         <v>0.834</v>
@@ -3359,7 +3359,7 @@
         <v>0.46</v>
       </c>
       <c r="J65">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="K65">
         <v>0.668</v>
@@ -3457,7 +3457,7 @@
         <v>0.671</v>
       </c>
       <c r="L67">
-        <v>0.6760000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="M67">
         <v>0.362</v>
@@ -3500,7 +3500,7 @@
         <v>0.86</v>
       </c>
       <c r="K68">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="L68">
         <v>0.697</v>
@@ -3522,7 +3522,7 @@
         <v>2016</v>
       </c>
       <c r="C69">
-        <v>0.9280000000000001</v>
+        <v>0.928</v>
       </c>
       <c r="D69">
         <v>0.8110000000000001</v>
@@ -3592,7 +3592,7 @@
         <v>0.788</v>
       </c>
       <c r="K70">
-        <v>0.692</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="L70">
         <v>0.529</v>
@@ -3632,7 +3632,7 @@
         <v>0.951</v>
       </c>
       <c r="I71">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J71">
         <v>0.92</v>
@@ -3663,7 +3663,7 @@
         <v>0.961</v>
       </c>
       <c r="D72">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E72">
         <v>0.907</v>
@@ -3681,7 +3681,7 @@
         <v>0.898</v>
       </c>
       <c r="J72">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="K72">
         <v>0.861</v>
@@ -3690,7 +3690,7 @@
         <v>0.766</v>
       </c>
       <c r="M72">
-        <v>0.5530000000000001</v>
+        <v>0.553</v>
       </c>
       <c r="N72">
         <v>0.387</v>
@@ -3718,7 +3718,7 @@
         <v>0.641</v>
       </c>
       <c r="G73">
-        <v>0.817</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="H73">
         <v>0.891</v>
@@ -3758,10 +3758,10 @@
         <v>0.883</v>
       </c>
       <c r="E74">
-        <v>0.94</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F74">
-        <v>0.816</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G74">
         <v>0.921</v>
@@ -3776,7 +3776,7 @@
         <v>0.828</v>
       </c>
       <c r="K74">
-        <v>0.815</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="L74">
         <v>0.734</v>
@@ -3871,7 +3871,7 @@
         <v>0.782</v>
       </c>
       <c r="L76">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M76">
         <v>0.5629999999999999</v>
@@ -3902,7 +3902,7 @@
         <v>0.887</v>
       </c>
       <c r="G77">
-        <v>0.8020000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="H77">
         <v>0.791</v>
@@ -3942,7 +3942,7 @@
         <v>0.827</v>
       </c>
       <c r="E78">
-        <v>0.8010000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="F78">
         <v>0.821</v>
@@ -3960,10 +3960,10 @@
         <v>0.849</v>
       </c>
       <c r="K78">
-        <v>0.8050000000000001</v>
+        <v>0.805</v>
       </c>
       <c r="L78">
-        <v>0.6800000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="M78">
         <v>0.454</v>
@@ -3988,7 +3988,7 @@
         <v>0.8080000000000001</v>
       </c>
       <c r="E79">
-        <v>0.814</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="F79">
         <v>0.836</v>
@@ -4031,7 +4031,7 @@
         <v>0.985</v>
       </c>
       <c r="D80">
-        <v>0.9310000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="E80">
         <v>0.872</v>
@@ -4098,7 +4098,7 @@
         <v>0.534</v>
       </c>
       <c r="K81">
-        <v>0.693</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="L81">
         <v>0.536</v>
@@ -4193,7 +4193,7 @@
         <v>0.57</v>
       </c>
       <c r="L83">
-        <v>0.5560000000000001</v>
+        <v>0.556</v>
       </c>
       <c r="M83">
         <v>0.344</v>
@@ -4399,13 +4399,13 @@
         <v>0.949</v>
       </c>
       <c r="D88">
-        <v>0.9260000000000001</v>
+        <v>0.926</v>
       </c>
       <c r="E88">
         <v>0.9330000000000001</v>
       </c>
       <c r="F88">
-        <v>0.564</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G88">
         <v>0.949</v>
@@ -4414,7 +4414,7 @@
         <v>0.973</v>
       </c>
       <c r="I88">
-        <v>0.9300000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="J88">
         <v>0.825</v>
@@ -4506,7 +4506,7 @@
         <v>0.779</v>
       </c>
       <c r="I90">
-        <v>0.818</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="J90">
         <v>0.772</v>
@@ -4515,7 +4515,7 @@
         <v>0.899</v>
       </c>
       <c r="L90">
-        <v>0.6810000000000001</v>
+        <v>0.681</v>
       </c>
       <c r="M90">
         <v>0.595</v>

</xml_diff>